<commit_message>
Changed calibration targets for HPV and modified assortativity parameters.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicktzr\Google Drive\ICRC\CISNET\Model\HHCoM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msharma1\Documents\HHCoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Screening and Treatment" sheetId="5" r:id="rId6"/>
     <sheet name="Cervical Cancer" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="305">
   <si>
     <t>N</t>
   </si>
@@ -930,6 +930,21 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>17-19</t>
+  </si>
+  <si>
+    <t>55-65</t>
+  </si>
+  <si>
+    <t>HPV Prevalence in HIV+ Women (all)</t>
+  </si>
+  <si>
+    <t>McDonald</t>
+  </si>
+  <si>
+    <t>HPV Prevalence in HIV- Women (all)</t>
   </si>
 </sst>
 </file>
@@ -1549,8 +1564,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I143" totalsRowShown="0">
-  <autoFilter ref="A1:I143"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I161" totalsRowShown="0">
+  <autoFilter ref="A1:I161"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Criteria"/>
     <tableColumn id="9" name="Source"/>
@@ -1901,10 +1916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M143"/>
+  <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5550,6 +5565,474 @@
       </c>
       <c r="H143" s="77"/>
       <c r="I143" s="77"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>302</v>
+      </c>
+      <c r="B144" t="s">
+        <v>303</v>
+      </c>
+      <c r="C144" t="s">
+        <v>300</v>
+      </c>
+      <c r="D144">
+        <v>2014</v>
+      </c>
+      <c r="E144">
+        <v>36</v>
+      </c>
+      <c r="F144">
+        <v>48</v>
+      </c>
+      <c r="G144" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.75</v>
+      </c>
+      <c r="H144" s="77"/>
+      <c r="I144" s="77"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>302</v>
+      </c>
+      <c r="B145" t="s">
+        <v>303</v>
+      </c>
+      <c r="C145" t="s">
+        <v>85</v>
+      </c>
+      <c r="D145">
+        <v>2014</v>
+      </c>
+      <c r="E145">
+        <v>134</v>
+      </c>
+      <c r="F145">
+        <v>221</v>
+      </c>
+      <c r="G145" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.60633484162895923</v>
+      </c>
+      <c r="H145" s="77"/>
+      <c r="I145" s="77"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>302</v>
+      </c>
+      <c r="B146" t="s">
+        <v>303</v>
+      </c>
+      <c r="C146" t="s">
+        <v>86</v>
+      </c>
+      <c r="D146">
+        <v>2014</v>
+      </c>
+      <c r="E146">
+        <v>145</v>
+      </c>
+      <c r="F146">
+        <v>243</v>
+      </c>
+      <c r="G146" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.5967078189300411</v>
+      </c>
+      <c r="H146" s="77"/>
+      <c r="I146" s="77"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>302</v>
+      </c>
+      <c r="B147" t="s">
+        <v>303</v>
+      </c>
+      <c r="C147" t="s">
+        <v>87</v>
+      </c>
+      <c r="D147">
+        <v>2014</v>
+      </c>
+      <c r="E147">
+        <v>96</v>
+      </c>
+      <c r="F147">
+        <v>175</v>
+      </c>
+      <c r="G147" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.5485714285714286</v>
+      </c>
+      <c r="H147" s="77"/>
+      <c r="I147" s="77"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>302</v>
+      </c>
+      <c r="B148" t="s">
+        <v>303</v>
+      </c>
+      <c r="C148" t="s">
+        <v>88</v>
+      </c>
+      <c r="D148">
+        <v>2014</v>
+      </c>
+      <c r="E148">
+        <v>189</v>
+      </c>
+      <c r="F148">
+        <v>407</v>
+      </c>
+      <c r="G148" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.46437346437346438</v>
+      </c>
+      <c r="H148" s="77"/>
+      <c r="I148" s="77"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>302</v>
+      </c>
+      <c r="B149" t="s">
+        <v>303</v>
+      </c>
+      <c r="C149" t="s">
+        <v>89</v>
+      </c>
+      <c r="D149">
+        <v>2014</v>
+      </c>
+      <c r="E149">
+        <v>62</v>
+      </c>
+      <c r="F149">
+        <v>147</v>
+      </c>
+      <c r="G149" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.42176870748299322</v>
+      </c>
+      <c r="H149" s="77"/>
+      <c r="I149" s="77"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>302</v>
+      </c>
+      <c r="B150" t="s">
+        <v>303</v>
+      </c>
+      <c r="C150" t="s">
+        <v>90</v>
+      </c>
+      <c r="D150">
+        <v>2014</v>
+      </c>
+      <c r="E150">
+        <v>33</v>
+      </c>
+      <c r="F150">
+        <v>76</v>
+      </c>
+      <c r="G150" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.43421052631578949</v>
+      </c>
+      <c r="H150" s="77"/>
+      <c r="I150" s="77"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>302</v>
+      </c>
+      <c r="B151" t="s">
+        <v>303</v>
+      </c>
+      <c r="C151" t="s">
+        <v>91</v>
+      </c>
+      <c r="D151">
+        <v>2014</v>
+      </c>
+      <c r="E151">
+        <v>15</v>
+      </c>
+      <c r="F151">
+        <v>28</v>
+      </c>
+      <c r="G151" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="H151" s="77"/>
+      <c r="I151" s="77"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>302</v>
+      </c>
+      <c r="B152" t="s">
+        <v>303</v>
+      </c>
+      <c r="C152" t="s">
+        <v>301</v>
+      </c>
+      <c r="D152">
+        <v>2014</v>
+      </c>
+      <c r="E152">
+        <v>9</v>
+      </c>
+      <c r="F152">
+        <v>26</v>
+      </c>
+      <c r="G152" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.34615384615384615</v>
+      </c>
+      <c r="H152" s="77"/>
+      <c r="I152" s="77"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>304</v>
+      </c>
+      <c r="B153" t="s">
+        <v>303</v>
+      </c>
+      <c r="C153" t="s">
+        <v>300</v>
+      </c>
+      <c r="D153">
+        <v>2014</v>
+      </c>
+      <c r="E153">
+        <v>115</v>
+      </c>
+      <c r="F153">
+        <v>191</v>
+      </c>
+      <c r="G153" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.60209424083769636</v>
+      </c>
+      <c r="H153" s="77"/>
+      <c r="I153" s="77"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>304</v>
+      </c>
+      <c r="B154" t="s">
+        <v>303</v>
+      </c>
+      <c r="C154" t="s">
+        <v>85</v>
+      </c>
+      <c r="D154">
+        <v>2014</v>
+      </c>
+      <c r="E154">
+        <v>261</v>
+      </c>
+      <c r="F154">
+        <v>693</v>
+      </c>
+      <c r="G154" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.37662337662337664</v>
+      </c>
+      <c r="H154" s="77"/>
+      <c r="I154" s="77"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>304</v>
+      </c>
+      <c r="B155" t="s">
+        <v>303</v>
+      </c>
+      <c r="C155" t="s">
+        <v>86</v>
+      </c>
+      <c r="D155">
+        <v>2014</v>
+      </c>
+      <c r="E155">
+        <v>158</v>
+      </c>
+      <c r="F155">
+        <v>662</v>
+      </c>
+      <c r="G155" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.23867069486404835</v>
+      </c>
+      <c r="H155" s="77"/>
+      <c r="I155" s="77"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>304</v>
+      </c>
+      <c r="B156" t="s">
+        <v>303</v>
+      </c>
+      <c r="C156" t="s">
+        <v>87</v>
+      </c>
+      <c r="D156">
+        <v>2014</v>
+      </c>
+      <c r="E156">
+        <v>135</v>
+      </c>
+      <c r="F156">
+        <v>666</v>
+      </c>
+      <c r="G156" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.20270270270270271</v>
+      </c>
+      <c r="H156" s="77"/>
+      <c r="I156" s="77"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>304</v>
+      </c>
+      <c r="B157" t="s">
+        <v>303</v>
+      </c>
+      <c r="C157" t="s">
+        <v>88</v>
+      </c>
+      <c r="D157">
+        <v>2014</v>
+      </c>
+      <c r="E157">
+        <v>439</v>
+      </c>
+      <c r="F157">
+        <v>2272</v>
+      </c>
+      <c r="G157" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.1932218309859155</v>
+      </c>
+      <c r="H157" s="77"/>
+      <c r="I157" s="77"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>304</v>
+      </c>
+      <c r="B158" t="s">
+        <v>303</v>
+      </c>
+      <c r="C158" t="s">
+        <v>89</v>
+      </c>
+      <c r="D158">
+        <v>2014</v>
+      </c>
+      <c r="E158">
+        <v>247</v>
+      </c>
+      <c r="F158">
+        <v>1400</v>
+      </c>
+      <c r="G158" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.17642857142857143</v>
+      </c>
+      <c r="H158" s="77"/>
+      <c r="I158" s="77"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>304</v>
+      </c>
+      <c r="B159" t="s">
+        <v>303</v>
+      </c>
+      <c r="C159" t="s">
+        <v>90</v>
+      </c>
+      <c r="D159">
+        <v>2014</v>
+      </c>
+      <c r="E159">
+        <v>130</v>
+      </c>
+      <c r="F159">
+        <v>982</v>
+      </c>
+      <c r="G159" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.13238289205702647</v>
+      </c>
+      <c r="H159" s="77"/>
+      <c r="I159" s="77"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>304</v>
+      </c>
+      <c r="B160" t="s">
+        <v>303</v>
+      </c>
+      <c r="C160" t="s">
+        <v>91</v>
+      </c>
+      <c r="D160">
+        <v>2014</v>
+      </c>
+      <c r="E160">
+        <v>102</v>
+      </c>
+      <c r="F160">
+        <v>617</v>
+      </c>
+      <c r="G160" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.16531604538087522</v>
+      </c>
+      <c r="H160" s="77"/>
+      <c r="I160" s="77"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>304</v>
+      </c>
+      <c r="B161" t="s">
+        <v>303</v>
+      </c>
+      <c r="C161" t="s">
+        <v>301</v>
+      </c>
+      <c r="D161">
+        <v>2014</v>
+      </c>
+      <c r="E161">
+        <v>83</v>
+      </c>
+      <c r="F161">
+        <v>567</v>
+      </c>
+      <c r="G161" s="76">
+        <f>Table1[Pos]/Table1[N]</f>
+        <v>0.14638447971781304</v>
+      </c>
+      <c r="H161" s="77"/>
+      <c r="I161" s="77"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated likelihood function to use latest data.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msharma1\Documents\HHCoM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="306">
   <si>
     <t>N</t>
   </si>
@@ -945,6 +945,9 @@
   </si>
   <si>
     <t>HPV Prevalence in HIV- Women (all)</t>
+  </si>
+  <si>
+    <t>McDonald 2014</t>
   </si>
 </sst>
 </file>
@@ -1852,50 +1855,49 @@
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1918,19 +1920,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="F162" sqref="F162"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="5" width="11.90625" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1962,18 +1964,18 @@
         <v>283</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>257</v>
       </c>
       <c r="D2" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E2" s="21">
         <v>6</v>
@@ -1989,18 +1991,18 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>258</v>
       </c>
       <c r="D3" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E3" s="21">
         <v>12</v>
@@ -2016,18 +2018,18 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>259</v>
       </c>
       <c r="D4" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E4" s="21">
         <v>31</v>
@@ -2040,18 +2042,18 @@
         <v>0.12757201646090535</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>260</v>
       </c>
       <c r="D5" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E5" s="21">
         <v>27</v>
@@ -2064,18 +2066,18 @@
         <v>0.15428571428571428</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>261</v>
       </c>
       <c r="D6" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E6" s="21">
         <v>33</v>
@@ -2088,18 +2090,18 @@
         <v>8.1081081081081086E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>262</v>
       </c>
       <c r="D7" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E7" s="21">
         <v>8</v>
@@ -2112,18 +2114,18 @@
         <v>5.4421768707482991E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>263</v>
       </c>
       <c r="D8" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E8" s="21">
         <v>6</v>
@@ -2136,18 +2138,18 @@
         <v>7.8947368421052627E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>264</v>
       </c>
       <c r="D9" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E9" s="21">
         <v>2</v>
@@ -2160,18 +2162,18 @@
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>265</v>
       </c>
       <c r="D10" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E10" s="21">
         <v>1</v>
@@ -2185,18 +2187,18 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>267</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>266</v>
       </c>
       <c r="D11" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E11" s="21">
         <v>1</v>
@@ -2210,18 +2212,18 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>257</v>
       </c>
       <c r="D12" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E12" s="21">
         <v>3</v>
@@ -2234,18 +2236,18 @@
         <v>1.5706806282722512E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>258</v>
       </c>
       <c r="D13" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E13" s="21">
         <v>19</v>
@@ -2258,18 +2260,18 @@
         <v>2.7417027417027416E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>259</v>
       </c>
       <c r="D14" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E14" s="21">
         <v>14</v>
@@ -2282,18 +2284,18 @@
         <v>2.1148036253776436E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>260</v>
       </c>
       <c r="D15" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E15" s="21">
         <v>24</v>
@@ -2306,18 +2308,18 @@
         <v>3.6036036036036036E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>261</v>
       </c>
       <c r="D16" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E16" s="21">
         <v>65</v>
@@ -2330,18 +2332,18 @@
         <v>2.8609154929577465E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>262</v>
       </c>
       <c r="D17" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E17" s="21">
         <v>44</v>
@@ -2354,18 +2356,18 @@
         <v>3.1428571428571431E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>263</v>
       </c>
       <c r="D18" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E18" s="21">
         <v>30</v>
@@ -2378,18 +2380,18 @@
         <v>3.0549898167006109E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>264</v>
       </c>
       <c r="D19" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E19" s="21">
         <v>13</v>
@@ -2402,18 +2404,18 @@
         <v>2.1069692058346839E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>265</v>
       </c>
       <c r="D20" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E20" s="21">
         <v>4</v>
@@ -2427,18 +2429,18 @@
         <v>1.4109347442680775E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>268</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>266</v>
       </c>
       <c r="D21" s="21">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="E21" s="21">
         <v>4</v>
@@ -2452,7 +2454,7 @@
         <v>1.4109347442680775E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>269</v>
       </c>
@@ -2476,7 +2478,7 @@
         <v>0.16317991631799164</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>269</v>
       </c>
@@ -2500,7 +2502,7 @@
         <v>0.20787746170678337</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>269</v>
       </c>
@@ -2524,7 +2526,7 @@
         <v>0.21878453038674034</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>269</v>
       </c>
@@ -2548,7 +2550,7 @@
         <v>0.14744351961950058</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>269</v>
       </c>
@@ -2572,7 +2574,7 @@
         <v>0.11534154535274356</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>269</v>
       </c>
@@ -2596,7 +2598,7 @@
         <v>6.1409179056237877E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>269</v>
       </c>
@@ -2620,7 +2622,7 @@
         <v>3.780718336483932E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>269</v>
       </c>
@@ -2644,7 +2646,7 @@
         <v>2.0155038759689922E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>269</v>
       </c>
@@ -2668,7 +2670,7 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>269</v>
       </c>
@@ -2692,7 +2694,7 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>270</v>
       </c>
@@ -2716,7 +2718,7 @@
         <v>0.16317991631799164</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>270</v>
       </c>
@@ -2740,7 +2742,7 @@
         <v>0.20787746170678337</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>270</v>
       </c>
@@ -2764,7 +2766,7 @@
         <v>0.21878453038674034</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>270</v>
       </c>
@@ -2788,7 +2790,7 @@
         <v>0.14744351961950058</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>270</v>
       </c>
@@ -2812,7 +2814,7 @@
         <v>0.11534154535274356</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>270</v>
       </c>
@@ -2836,7 +2838,7 @@
         <v>6.1409179056237877E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>270</v>
       </c>
@@ -2860,7 +2862,7 @@
         <v>3.780718336483932E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>270</v>
       </c>
@@ -2884,7 +2886,7 @@
         <v>2.0155038759689922E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>270</v>
       </c>
@@ -2908,7 +2910,7 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>270</v>
       </c>
@@ -2932,7 +2934,7 @@
         <v>2.6981450252951095E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>271</v>
       </c>
@@ -2956,7 +2958,7 @@
         <v>0.58638743455497377</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>271</v>
       </c>
@@ -2980,7 +2982,7 @@
         <v>0.34920634920634919</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>271</v>
       </c>
@@ -3004,7 +3006,7 @@
         <v>0.2175226586102719</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>271</v>
       </c>
@@ -3028,7 +3030,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
         <v>271</v>
       </c>
@@ -3052,7 +3054,7 @@
         <v>0.16461267605633803</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>271</v>
       </c>
@@ -3076,7 +3078,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>271</v>
       </c>
@@ -3100,7 +3102,7 @@
         <v>0.10183299389002037</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>271</v>
       </c>
@@ -3126,7 +3128,7 @@
       <c r="H49" s="21"/>
       <c r="I49" s="21"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>271</v>
       </c>
@@ -3152,7 +3154,7 @@
       <c r="H50" s="21"/>
       <c r="I50" s="21"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>271</v>
       </c>
@@ -3178,7 +3180,7 @@
       <c r="H51" s="21"/>
       <c r="I51" s="21"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>274</v>
       </c>
@@ -3206,7 +3208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>274</v>
       </c>
@@ -3234,7 +3236,7 @@
         <v>0.73896528627634828</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>274</v>
       </c>
@@ -3262,7 +3264,7 @@
         <v>0.62062966115974605</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="21" t="s">
         <v>274</v>
       </c>
@@ -3290,7 +3292,7 @@
         <v>0.47893264233014488</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="21" t="s">
         <v>280</v>
       </c>
@@ -3318,7 +3320,7 @@
         <v>0.59252264082678208</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="21" t="s">
         <v>280</v>
       </c>
@@ -3346,7 +3348,7 @@
         <v>0.32293097813833699</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>280</v>
       </c>
@@ -3374,7 +3376,7 @@
         <v>0.29832234128895085</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
         <v>280</v>
       </c>
@@ -3402,7 +3404,7 @@
         <v>0.27445149548815129</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
         <v>287</v>
       </c>
@@ -3426,7 +3428,7 @@
         <v>1.0135135135135136E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
         <v>287</v>
       </c>
@@ -3450,7 +3452,7 @@
         <v>8.8504182065745965E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="21" t="s">
         <v>287</v>
       </c>
@@ -3474,7 +3476,7 @@
         <v>0.28191051331320338</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
         <v>287</v>
       </c>
@@ -3498,7 +3500,7 @@
         <v>0.45185719437432381</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
         <v>287</v>
       </c>
@@ -3522,7 +3524,7 @@
         <v>0.3721881390593047</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
         <v>287</v>
       </c>
@@ -3546,7 +3548,7 @@
         <v>0.26923076923076922</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
         <v>287</v>
       </c>
@@ -3570,7 +3572,7 @@
         <v>0.22687224669603523</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
         <v>288</v>
       </c>
@@ -3594,7 +3596,7 @@
         <v>1.3157894736842105E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
         <v>288</v>
       </c>
@@ -3618,7 +3620,7 @@
         <v>0.10095312196070803</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
         <v>288</v>
       </c>
@@ -3642,7 +3644,7 @@
         <v>0.33324183365358223</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
         <v>288</v>
       </c>
@@ -3668,7 +3670,7 @@
       <c r="H70" s="77"/>
       <c r="I70" s="77"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
         <v>288</v>
       </c>
@@ -3694,7 +3696,7 @@
       <c r="H71" s="77"/>
       <c r="I71" s="77"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
         <v>288</v>
       </c>
@@ -3720,7 +3722,7 @@
       <c r="H72" s="77"/>
       <c r="I72" s="77"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
         <v>288</v>
       </c>
@@ -3746,7 +3748,7 @@
       <c r="H73" s="77"/>
       <c r="I73" s="77"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="21" t="s">
         <v>289</v>
       </c>
@@ -3772,7 +3774,7 @@
       <c r="H74" s="77"/>
       <c r="I74" s="77"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="21" t="s">
         <v>289</v>
       </c>
@@ -3798,7 +3800,7 @@
       <c r="H75" s="77"/>
       <c r="I75" s="77"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
         <v>289</v>
       </c>
@@ -3824,7 +3826,7 @@
       <c r="H76" s="77"/>
       <c r="I76" s="77"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
         <v>289</v>
       </c>
@@ -3850,7 +3852,7 @@
       <c r="H77" s="77"/>
       <c r="I77" s="77"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
         <v>289</v>
       </c>
@@ -3876,7 +3878,7 @@
       <c r="H78" s="77"/>
       <c r="I78" s="77"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
         <v>289</v>
       </c>
@@ -3902,7 +3904,7 @@
       <c r="H79" s="77"/>
       <c r="I79" s="77"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="21" t="s">
         <v>289</v>
       </c>
@@ -3928,7 +3930,7 @@
       <c r="H80" s="77"/>
       <c r="I80" s="77"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="21" t="s">
         <v>290</v>
       </c>
@@ -3954,7 +3956,7 @@
       <c r="H81" s="77"/>
       <c r="I81" s="77"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="21" t="s">
         <v>290</v>
       </c>
@@ -3980,7 +3982,7 @@
       <c r="H82" s="77"/>
       <c r="I82" s="77"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
         <v>290</v>
       </c>
@@ -4006,7 +4008,7 @@
       <c r="H83" s="77"/>
       <c r="I83" s="77"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="21" t="s">
         <v>290</v>
       </c>
@@ -4032,7 +4034,7 @@
       <c r="H84" s="77"/>
       <c r="I84" s="77"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="21" t="s">
         <v>290</v>
       </c>
@@ -4058,7 +4060,7 @@
       <c r="H85" s="77"/>
       <c r="I85" s="77"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="21" t="s">
         <v>290</v>
       </c>
@@ -4084,7 +4086,7 @@
       <c r="H86" s="77"/>
       <c r="I86" s="77"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="21" t="s">
         <v>290</v>
       </c>
@@ -4110,7 +4112,7 @@
       <c r="H87" s="77"/>
       <c r="I87" s="77"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="21" t="s">
         <v>291</v>
       </c>
@@ -4136,7 +4138,7 @@
       <c r="H88" s="77"/>
       <c r="I88" s="77"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="21" t="s">
         <v>291</v>
       </c>
@@ -4162,7 +4164,7 @@
       <c r="H89" s="77"/>
       <c r="I89" s="77"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="21" t="s">
         <v>291</v>
       </c>
@@ -4188,7 +4190,7 @@
       <c r="H90" s="77"/>
       <c r="I90" s="77"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="21" t="s">
         <v>291</v>
       </c>
@@ -4214,7 +4216,7 @@
       <c r="H91" s="77"/>
       <c r="I91" s="77"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="21" t="s">
         <v>291</v>
       </c>
@@ -4240,7 +4242,7 @@
       <c r="H92" s="77"/>
       <c r="I92" s="77"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="21" t="s">
         <v>291</v>
       </c>
@@ -4266,7 +4268,7 @@
       <c r="H93" s="77"/>
       <c r="I93" s="77"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="21" t="s">
         <v>291</v>
       </c>
@@ -4292,7 +4294,7 @@
       <c r="H94" s="77"/>
       <c r="I94" s="77"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
         <v>292</v>
       </c>
@@ -4318,7 +4320,7 @@
       <c r="H95" s="77"/>
       <c r="I95" s="77"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="21" t="s">
         <v>292</v>
       </c>
@@ -4344,7 +4346,7 @@
       <c r="H96" s="77"/>
       <c r="I96" s="77"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="21" t="s">
         <v>292</v>
       </c>
@@ -4370,7 +4372,7 @@
       <c r="H97" s="77"/>
       <c r="I97" s="77"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="21" t="s">
         <v>292</v>
       </c>
@@ -4396,7 +4398,7 @@
       <c r="H98" s="77"/>
       <c r="I98" s="77"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="21" t="s">
         <v>292</v>
       </c>
@@ -4422,7 +4424,7 @@
       <c r="H99" s="77"/>
       <c r="I99" s="77"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="21" t="s">
         <v>292</v>
       </c>
@@ -4448,7 +4450,7 @@
       <c r="H100" s="77"/>
       <c r="I100" s="77"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
         <v>292</v>
       </c>
@@ -4474,7 +4476,7 @@
       <c r="H101" s="77"/>
       <c r="I101" s="77"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="21" t="s">
         <v>293</v>
       </c>
@@ -4500,7 +4502,7 @@
       <c r="H102" s="77"/>
       <c r="I102" s="77"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="21" t="s">
         <v>293</v>
       </c>
@@ -4526,7 +4528,7 @@
       <c r="H103" s="77"/>
       <c r="I103" s="77"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="21" t="s">
         <v>293</v>
       </c>
@@ -4552,7 +4554,7 @@
       <c r="H104" s="77"/>
       <c r="I104" s="77"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="21" t="s">
         <v>293</v>
       </c>
@@ -4578,7 +4580,7 @@
       <c r="H105" s="77"/>
       <c r="I105" s="77"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="21" t="s">
         <v>293</v>
       </c>
@@ -4604,7 +4606,7 @@
       <c r="H106" s="77"/>
       <c r="I106" s="77"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="21" t="s">
         <v>293</v>
       </c>
@@ -4630,7 +4632,7 @@
       <c r="H107" s="77"/>
       <c r="I107" s="77"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="21" t="s">
         <v>293</v>
       </c>
@@ -4656,7 +4658,7 @@
       <c r="H108" s="77"/>
       <c r="I108" s="77"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="21" t="s">
         <v>294</v>
       </c>
@@ -4682,7 +4684,7 @@
       <c r="H109" s="77"/>
       <c r="I109" s="77"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="21" t="s">
         <v>294</v>
       </c>
@@ -4708,7 +4710,7 @@
       <c r="H110" s="77"/>
       <c r="I110" s="77"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="21" t="s">
         <v>294</v>
       </c>
@@ -4734,7 +4736,7 @@
       <c r="H111" s="77"/>
       <c r="I111" s="77"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="21" t="s">
         <v>294</v>
       </c>
@@ -4760,7 +4762,7 @@
       <c r="H112" s="77"/>
       <c r="I112" s="77"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="21" t="s">
         <v>294</v>
       </c>
@@ -4786,7 +4788,7 @@
       <c r="H113" s="77"/>
       <c r="I113" s="77"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="21" t="s">
         <v>294</v>
       </c>
@@ -4812,7 +4814,7 @@
       <c r="H114" s="77"/>
       <c r="I114" s="77"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="21" t="s">
         <v>294</v>
       </c>
@@ -4838,7 +4840,7 @@
       <c r="H115" s="77"/>
       <c r="I115" s="77"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="21" t="s">
         <v>295</v>
       </c>
@@ -4864,7 +4866,7 @@
       <c r="H116" s="77"/>
       <c r="I116" s="77"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="21" t="s">
         <v>295</v>
       </c>
@@ -4890,7 +4892,7 @@
       <c r="H117" s="77"/>
       <c r="I117" s="77"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="21" t="s">
         <v>295</v>
       </c>
@@ -4916,7 +4918,7 @@
       <c r="H118" s="77"/>
       <c r="I118" s="77"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="21" t="s">
         <v>295</v>
       </c>
@@ -4942,7 +4944,7 @@
       <c r="H119" s="77"/>
       <c r="I119" s="77"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="21" t="s">
         <v>295</v>
       </c>
@@ -4968,7 +4970,7 @@
       <c r="H120" s="77"/>
       <c r="I120" s="77"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="21" t="s">
         <v>295</v>
       </c>
@@ -4994,7 +4996,7 @@
       <c r="H121" s="77"/>
       <c r="I121" s="77"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="21" t="s">
         <v>295</v>
       </c>
@@ -5020,7 +5022,7 @@
       <c r="H122" s="77"/>
       <c r="I122" s="77"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="21" t="s">
         <v>296</v>
       </c>
@@ -5046,7 +5048,7 @@
       <c r="H123" s="77"/>
       <c r="I123" s="77"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="21" t="s">
         <v>296</v>
       </c>
@@ -5072,7 +5074,7 @@
       <c r="H124" s="77"/>
       <c r="I124" s="77"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="21" t="s">
         <v>296</v>
       </c>
@@ -5098,7 +5100,7 @@
       <c r="H125" s="77"/>
       <c r="I125" s="77"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="21" t="s">
         <v>296</v>
       </c>
@@ -5124,7 +5126,7 @@
       <c r="H126" s="77"/>
       <c r="I126" s="77"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="21" t="s">
         <v>296</v>
       </c>
@@ -5150,7 +5152,7 @@
       <c r="H127" s="77"/>
       <c r="I127" s="77"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="21" t="s">
         <v>296</v>
       </c>
@@ -5176,7 +5178,7 @@
       <c r="H128" s="77"/>
       <c r="I128" s="77"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="21" t="s">
         <v>296</v>
       </c>
@@ -5202,7 +5204,7 @@
       <c r="H129" s="77"/>
       <c r="I129" s="77"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="21" t="s">
         <v>297</v>
       </c>
@@ -5228,7 +5230,7 @@
       <c r="H130" s="77"/>
       <c r="I130" s="77"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="21" t="s">
         <v>297</v>
       </c>
@@ -5254,7 +5256,7 @@
       <c r="H131" s="77"/>
       <c r="I131" s="77"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="21" t="s">
         <v>297</v>
       </c>
@@ -5280,7 +5282,7 @@
       <c r="H132" s="77"/>
       <c r="I132" s="77"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="21" t="s">
         <v>297</v>
       </c>
@@ -5306,7 +5308,7 @@
       <c r="H133" s="77"/>
       <c r="I133" s="77"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="21" t="s">
         <v>297</v>
       </c>
@@ -5332,7 +5334,7 @@
       <c r="H134" s="77"/>
       <c r="I134" s="77"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="21" t="s">
         <v>297</v>
       </c>
@@ -5358,7 +5360,7 @@
       <c r="H135" s="77"/>
       <c r="I135" s="77"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="21" t="s">
         <v>297</v>
       </c>
@@ -5384,7 +5386,7 @@
       <c r="H136" s="77"/>
       <c r="I136" s="77"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="21" t="s">
         <v>298</v>
       </c>
@@ -5410,7 +5412,7 @@
       <c r="H137" s="77"/>
       <c r="I137" s="77"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="21" t="s">
         <v>298</v>
       </c>
@@ -5436,7 +5438,7 @@
       <c r="H138" s="77"/>
       <c r="I138" s="77"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="21" t="s">
         <v>298</v>
       </c>
@@ -5462,7 +5464,7 @@
       <c r="H139" s="77"/>
       <c r="I139" s="77"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="21" t="s">
         <v>298</v>
       </c>
@@ -5488,7 +5490,7 @@
       <c r="H140" s="77"/>
       <c r="I140" s="77"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="21" t="s">
         <v>298</v>
       </c>
@@ -5514,7 +5516,7 @@
       <c r="H141" s="77"/>
       <c r="I141" s="77"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="21" t="s">
         <v>298</v>
       </c>
@@ -5540,7 +5542,7 @@
       <c r="H142" s="77"/>
       <c r="I142" s="77"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="21" t="s">
         <v>298</v>
       </c>
@@ -5566,7 +5568,7 @@
       <c r="H143" s="77"/>
       <c r="I143" s="77"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>302</v>
       </c>
@@ -5592,7 +5594,7 @@
       <c r="H144" s="77"/>
       <c r="I144" s="77"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>302</v>
       </c>
@@ -5618,7 +5620,7 @@
       <c r="H145" s="77"/>
       <c r="I145" s="77"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>302</v>
       </c>
@@ -5644,7 +5646,7 @@
       <c r="H146" s="77"/>
       <c r="I146" s="77"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>302</v>
       </c>
@@ -5670,7 +5672,7 @@
       <c r="H147" s="77"/>
       <c r="I147" s="77"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>302</v>
       </c>
@@ -5696,7 +5698,7 @@
       <c r="H148" s="77"/>
       <c r="I148" s="77"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>302</v>
       </c>
@@ -5722,7 +5724,7 @@
       <c r="H149" s="77"/>
       <c r="I149" s="77"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>302</v>
       </c>
@@ -5748,7 +5750,7 @@
       <c r="H150" s="77"/>
       <c r="I150" s="77"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>302</v>
       </c>
@@ -5774,7 +5776,7 @@
       <c r="H151" s="77"/>
       <c r="I151" s="77"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>302</v>
       </c>
@@ -5800,7 +5802,7 @@
       <c r="H152" s="77"/>
       <c r="I152" s="77"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>304</v>
       </c>
@@ -5826,7 +5828,7 @@
       <c r="H153" s="77"/>
       <c r="I153" s="77"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>304</v>
       </c>
@@ -5852,7 +5854,7 @@
       <c r="H154" s="77"/>
       <c r="I154" s="77"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>304</v>
       </c>
@@ -5878,7 +5880,7 @@
       <c r="H155" s="77"/>
       <c r="I155" s="77"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>304</v>
       </c>
@@ -5904,7 +5906,7 @@
       <c r="H156" s="77"/>
       <c r="I156" s="77"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>304</v>
       </c>
@@ -5930,7 +5932,7 @@
       <c r="H157" s="77"/>
       <c r="I157" s="77"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>304</v>
       </c>
@@ -5956,7 +5958,7 @@
       <c r="H158" s="77"/>
       <c r="I158" s="77"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>304</v>
       </c>
@@ -5982,7 +5984,7 @@
       <c r="H159" s="77"/>
       <c r="I159" s="77"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>304</v>
       </c>
@@ -6008,7 +6010,7 @@
       <c r="H160" s="77"/>
       <c r="I160" s="77"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>304</v>
       </c>
@@ -6050,7 +6052,7 @@
       <selection activeCell="E12" sqref="E12:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6064,19 +6066,19 @@
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.453125" customWidth="1"/>
-    <col min="7" max="7" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="16" max="16" width="15.54296875" customWidth="1"/>
-    <col min="17" max="18" width="49.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.54296875" customWidth="1"/>
-    <col min="21" max="21" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="18" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>191</v>
       </c>
@@ -6087,7 +6089,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>194</v>
       </c>
@@ -6137,7 +6139,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="35">
         <v>16</v>
       </c>
@@ -6187,7 +6189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="35">
         <v>18</v>
       </c>
@@ -6237,7 +6239,7 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="35">
         <v>31</v>
       </c>
@@ -6285,7 +6287,7 @@
         <v>8.08</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="58">
         <v>33</v>
       </c>
@@ -6332,7 +6334,7 @@
         <v>14.04</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="35"/>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
@@ -6365,7 +6367,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35">
         <v>39</v>
       </c>
@@ -6406,7 +6408,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="35">
         <v>51</v>
       </c>
@@ -6420,7 +6422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="35">
         <v>56</v>
       </c>
@@ -6437,7 +6439,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G11" s="33" t="s">
         <v>214</v>
       </c>
@@ -6454,7 +6456,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
         <v>194</v>
       </c>
@@ -6493,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>216</v>
       </c>
@@ -6536,7 +6538,7 @@
         <v>0.24271844660194175</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>219</v>
       </c>
@@ -6579,7 +6581,7 @@
         <v>0.12376237623762376</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>222</v>
       </c>
@@ -6611,7 +6613,7 @@
         <v>7.1225071225071226E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G16" s="35" t="s">
         <v>224</v>
       </c>
@@ -6625,7 +6627,7 @@
         <v>1.7130000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G17" s="58" t="s">
         <v>225</v>
       </c>
@@ -6639,7 +6641,7 @@
         <v>1.863</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="58" t="s">
         <v>226</v>
       </c>
@@ -6656,7 +6658,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="63"/>
       <c r="B19" s="64" t="s">
         <v>228</v>
@@ -6679,7 +6681,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="21" t="s">
         <v>217</v>
@@ -6706,7 +6708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>105</v>
       </c>
@@ -6732,7 +6734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>100</v>
       </c>
@@ -6761,7 +6763,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>99</v>
       </c>
@@ -6795,7 +6797,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>98</v>
       </c>
@@ -6821,7 +6823,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G25" s="69" t="s">
         <v>241</v>
       </c>
@@ -6832,7 +6834,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G27" s="33" t="s">
         <v>243</v>
       </c>
@@ -6840,7 +6842,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>245</v>
       </c>
@@ -6854,7 +6856,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G29" s="35" t="s">
         <v>218</v>
       </c>
@@ -6878,7 +6880,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G30" s="35" t="s">
         <v>221</v>
       </c>
@@ -6902,7 +6904,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G31" s="58" t="s">
         <v>249</v>
       </c>
@@ -6927,7 +6929,7 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q32" t="s">
         <v>98</v>
       </c>
@@ -6935,7 +6937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G34" s="33" t="s">
         <v>251</v>
       </c>
@@ -6943,7 +6945,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G35" s="38" t="s">
         <v>194</v>
       </c>
@@ -6969,7 +6971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G36" s="35" t="s">
         <v>217</v>
       </c>
@@ -7002,7 +7004,7 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G37" s="35" t="s">
         <v>220</v>
       </c>
@@ -7035,7 +7037,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G38" s="35" t="s">
         <v>223</v>
       </c>
@@ -7056,7 +7058,7 @@
         <v>1.925E-2</v>
       </c>
     </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G39" s="35" t="s">
         <v>224</v>
       </c>
@@ -7070,7 +7072,7 @@
         <v>0.10199999999999999</v>
       </c>
     </row>
-    <row r="40" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G40" s="58" t="s">
         <v>225</v>
       </c>
@@ -7084,7 +7086,7 @@
         <v>0.128</v>
       </c>
     </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G41" s="58" t="s">
         <v>226</v>
       </c>
@@ -7098,7 +7100,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G42" s="58" t="s">
         <v>229</v>
       </c>
@@ -7126,10 +7128,10 @@
       <selection activeCell="K109" sqref="K109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:21" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:21" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -7194,7 +7196,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>37</v>
       </c>
@@ -7259,7 +7261,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -7282,7 +7284,7 @@
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
     </row>
-    <row r="5" spans="1:21" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>49</v>
       </c>
@@ -7347,7 +7349,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>70</v>
       </c>
@@ -7412,8 +7414,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -7469,7 +7471,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>(59-23)/(70-15) * (2.5 + 5 * ($T12-1)) + 23</f>
         <v>24.636363636363637</v>
@@ -7537,7 +7539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ref="A13:A22" si="0">(59-23)/(70-15) * (2.5 + 5 * ($T13-1)) + 23</f>
         <v>27.90909090909091</v>
@@ -7605,7 +7607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>31.18181818181818</v>
@@ -7673,7 +7675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>34.454545454545453</v>
@@ -7741,7 +7743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>37.727272727272727</v>
@@ -7809,7 +7811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -7877,7 +7879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>44.272727272727273</v>
@@ -7945,7 +7947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>47.545454545454547</v>
@@ -8013,7 +8015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>50.818181818181813</v>
@@ -8081,7 +8083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>54.090909090909093</v>
@@ -8149,7 +8151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>57.363636363636367</v>
@@ -8217,8 +8219,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="29" spans="1:20" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>49</v>
       </c>
@@ -8274,7 +8276,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>(79-37)/(70-15) * (2.5 + 5 * ($T30-1)) + 37</f>
         <v>38.909090909090907</v>
@@ -8342,7 +8344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" ref="A31:A40" si="8">(79-37)/(70-15) * (2.5 + 5 * ($T31-1)) + 37</f>
         <v>42.727272727272727</v>
@@ -8410,7 +8412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="8"/>
         <v>46.545454545454547</v>
@@ -8478,7 +8480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="8"/>
         <v>50.36363636363636</v>
@@ -8546,7 +8548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="8"/>
         <v>54.181818181818187</v>
@@ -8614,7 +8616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="8"/>
         <v>58</v>
@@ -8682,7 +8684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="8"/>
         <v>61.81818181818182</v>
@@ -8750,7 +8752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="8"/>
         <v>65.63636363636364</v>
@@ -8818,7 +8820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="8"/>
         <v>69.454545454545453</v>
@@ -8886,7 +8888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="8"/>
         <v>73.27272727272728</v>
@@ -8954,7 +8956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="8"/>
         <v>77.090909090909093</v>
@@ -9022,7 +9024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -9030,7 +9032,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="58" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>18</v>
       </c>
@@ -9074,7 +9076,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>15.40909090909091</v>
       </c>
@@ -9118,7 +9120,7 @@
         <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>20.227272727272727</v>
       </c>
@@ -9162,7 +9164,7 @@
         <v>0.54545454545454541</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>25.045454545454547</v>
       </c>
@@ -9206,7 +9208,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>29.863636363636363</v>
       </c>
@@ -9250,7 +9252,7 @@
         <v>1.2727272727272727</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>34.68181818181818</v>
       </c>
@@ -9294,7 +9296,7 @@
         <v>1.6363636363636362</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>39.5</v>
       </c>
@@ -9338,7 +9340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>44.318181818181813</v>
       </c>
@@ -9382,7 +9384,7 @@
         <v>2.3636363636363633</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>49.136363636363633</v>
       </c>
@@ -9426,7 +9428,7 @@
         <v>2.7272727272727271</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53.954545454545453</v>
       </c>
@@ -9470,7 +9472,7 @@
         <v>3.0909090909090908</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="58" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>51</v>
       </c>
@@ -9514,7 +9516,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>6.3181818181818183</v>
       </c>
@@ -9558,7 +9560,7 @@
         <v>1.2272727272727273</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6.9545454545454541</v>
       </c>
@@ -9602,7 +9604,7 @@
         <v>1.6818181818181819</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>7.5909090909090908</v>
       </c>
@@ -9646,7 +9648,7 @@
         <v>2.1363636363636367</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>8.2272727272727266</v>
       </c>
@@ -9690,7 +9692,7 @@
         <v>2.5909090909090908</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>8.8636363636363633</v>
       </c>
@@ -9734,7 +9736,7 @@
         <v>3.0454545454545454</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9.5</v>
       </c>
@@ -9778,7 +9780,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>10.136363636363637</v>
       </c>
@@ -9822,7 +9824,7 @@
         <v>3.9545454545454546</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>10.772727272727273</v>
       </c>
@@ -9866,7 +9868,7 @@
         <v>4.4090909090909092</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>11.409090909090908</v>
       </c>
@@ -9910,7 +9912,7 @@
         <v>4.8636363636363633</v>
       </c>
     </row>
-    <row r="70" spans="1:27" ht="58" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
         <v>18</v>
       </c>
@@ -9967,7 +9969,7 @@
       </c>
       <c r="AA70" s="15"/>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <v>63.590909090909093</v>
       </c>
@@ -10045,7 +10047,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <v>63.590909090909093</v>
       </c>
@@ -10123,7 +10125,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>63.590909090909093</v>
       </c>
@@ -10201,7 +10203,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <v>63.590909090909093</v>
       </c>
@@ -10279,7 +10281,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <v>58.772727272727273</v>
       </c>
@@ -10357,7 +10359,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <v>53.954545454545453</v>
       </c>
@@ -10435,7 +10437,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <v>49.13636363636364</v>
       </c>
@@ -10513,7 +10515,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <v>44.31818181818182</v>
       </c>
@@ -10591,7 +10593,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <v>39.5</v>
       </c>
@@ -10669,7 +10671,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <v>34.681818181818187</v>
       </c>
@@ -10747,7 +10749,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <v>29.863636363636367</v>
       </c>
@@ -10825,7 +10827,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <v>25.045454545454547</v>
       </c>
@@ -10903,7 +10905,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <v>20.227272727272727</v>
       </c>
@@ -10981,7 +10983,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <v>15.409090909090907</v>
       </c>
@@ -11059,7 +11061,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="86" spans="1:27" ht="58" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
         <v>24</v>
       </c>
@@ -11116,7 +11118,7 @@
       </c>
       <c r="AA86" s="15"/>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <v>4.9090909090909092</v>
       </c>
@@ -11194,7 +11196,7 @@
         <v>4.795454545454545</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <v>4.9090909090909092</v>
       </c>
@@ -11272,7 +11274,7 @@
         <v>4.3863636363636367</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <v>4.9090909090909092</v>
       </c>
@@ -11350,7 +11352,7 @@
         <v>3.9772727272727271</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <v>4.9090909090909092</v>
       </c>
@@ -11428,7 +11430,7 @@
         <v>3.5681818181818183</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <v>4.7272727272727275</v>
       </c>
@@ -11506,7 +11508,7 @@
         <v>3.1590909090909092</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <v>4.5454545454545459</v>
       </c>
@@ -11584,7 +11586,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <v>4.3636363636363633</v>
       </c>
@@ -11662,7 +11664,7 @@
         <v>2.3409090909090908</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" s="15">
         <v>4.1818181818181817</v>
       </c>
@@ -11740,7 +11742,7 @@
         <v>1.9318181818181817</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" s="15">
         <v>4</v>
       </c>
@@ -11818,7 +11820,7 @@
         <v>1.5227272727272729</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" s="15">
         <v>3.8181818181818183</v>
       </c>
@@ -11896,7 +11898,7 @@
         <v>1.1136363636363638</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="15">
         <v>3.6363636363636367</v>
       </c>
@@ -11974,7 +11976,7 @@
         <v>0.70454545454545459</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="15">
         <v>3.4545454545454546</v>
       </c>
@@ -12052,7 +12054,7 @@
         <v>0.70454545454545459</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" s="15">
         <v>3.2727272727272725</v>
       </c>
@@ -12130,7 +12132,7 @@
         <v>0.70454545454545459</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="15">
         <v>3.0909090909090908</v>
       </c>
@@ -12208,8 +12210,8 @@
         <v>0.70454545454545459</v>
       </c>
     </row>
-    <row r="101" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="102" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="16"/>
       <c r="B102" s="17"/>
       <c r="C102" s="18" t="s">
@@ -12227,7 +12229,7 @@
       </c>
       <c r="K102" s="15"/>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" s="20"/>
       <c r="B103" s="21"/>
       <c r="C103" s="22" t="s">
@@ -12247,7 +12249,7 @@
       </c>
       <c r="K103" s="15"/>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" s="20"/>
       <c r="B104" s="21"/>
       <c r="C104" s="22" t="s">
@@ -12267,7 +12269,7 @@
       </c>
       <c r="K104" s="15"/>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="20"/>
       <c r="B105" s="21"/>
       <c r="C105" s="22" t="s">
@@ -12287,7 +12289,7 @@
       </c>
       <c r="K105" s="15"/>
     </row>
-    <row r="106" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="25"/>
       <c r="B106" s="26"/>
       <c r="C106" s="27" t="s">
@@ -12307,7 +12309,7 @@
       </c>
       <c r="K106" s="15"/>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H107">
         <v>9</v>
       </c>
@@ -12319,7 +12321,7 @@
       </c>
       <c r="K107" s="15"/>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H108">
         <v>8</v>
       </c>
@@ -12331,7 +12333,7 @@
       </c>
       <c r="K108" s="15"/>
     </row>
-    <row r="109" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>102</v>
       </c>
@@ -12346,7 +12348,7 @@
       </c>
       <c r="K109" s="15"/>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" s="29" t="s">
         <v>98</v>
       </c>
@@ -12367,7 +12369,7 @@
       </c>
       <c r="K110" s="15"/>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="s">
         <v>99</v>
       </c>
@@ -12388,7 +12390,7 @@
       </c>
       <c r="K111" s="15"/>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" s="20" t="s">
         <v>100</v>
       </c>
@@ -12406,7 +12408,7 @@
       </c>
       <c r="K112" s="15"/>
     </row>
-    <row r="113" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="25" t="s">
         <v>105</v>
       </c>
@@ -12424,7 +12426,7 @@
       </c>
       <c r="K113" s="15"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H114">
         <v>2</v>
       </c>
@@ -12435,7 +12437,7 @@
         <v>1.2272727272727273</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>106</v>
       </c>
@@ -12449,7 +12451,7 @@
         <v>1.2272727272727273</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="29" t="s">
         <v>98</v>
       </c>
@@ -12460,7 +12462,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="s">
         <v>99</v>
       </c>
@@ -12471,7 +12473,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="s">
         <v>100</v>
       </c>
@@ -12482,7 +12484,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="25" t="s">
         <v>105</v>
       </c>
@@ -12493,7 +12495,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D120" s="33" t="s">
         <v>111</v>
       </c>
@@ -12512,27 +12514,27 @@
       <selection activeCell="AD33" sqref="AD33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" customWidth="1"/>
     <col min="10" max="10" width="36" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="38.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.1796875" customWidth="1"/>
-    <col min="20" max="23" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.6328125" customWidth="1"/>
+    <col min="13" max="13" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" customWidth="1"/>
+    <col min="20" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5703125" customWidth="1"/>
     <col min="26" max="26" width="32" customWidth="1"/>
-    <col min="27" max="29" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.453125" customWidth="1"/>
+    <col min="27" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="34" t="s">
         <v>112</v>
       </c>
@@ -12559,7 +12561,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>119</v>
       </c>
@@ -12614,7 +12616,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>128</v>
       </c>
@@ -12676,7 +12678,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>136</v>
       </c>
@@ -12732,7 +12734,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
         <v>140</v>
       </c>
@@ -12767,7 +12769,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B6" s="44"/>
       <c r="M6" s="35" t="s">
         <v>144</v>
@@ -12806,7 +12808,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="M7" s="42" t="s">
         <v>148</v>
       </c>
@@ -12837,7 +12839,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S8" s="42" t="s">
         <v>151</v>
       </c>
@@ -12862,7 +12864,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="Y9" s="42" t="s">
         <v>155</v>
       </c>
@@ -12870,12 +12872,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AD10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S11" s="33" t="s">
         <v>158</v>
       </c>
@@ -12886,7 +12888,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K12" s="44"/>
       <c r="T12" s="33" t="s">
         <v>125</v>
@@ -12903,7 +12905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S13" s="43" t="s">
         <v>131</v>
       </c>
@@ -12926,7 +12928,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S14" s="38" t="s">
         <v>138</v>
       </c>
@@ -12943,7 +12945,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S15" s="38" t="s">
         <v>142</v>
       </c>
@@ -12956,7 +12958,7 @@
       </c>
       <c r="W15" s="35"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S16" s="38" t="s">
         <v>145</v>
       </c>
@@ -12969,7 +12971,7 @@
       </c>
       <c r="W16" s="35"/>
     </row>
-    <row r="17" spans="19:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S17" s="38" t="s">
         <v>149</v>
       </c>
@@ -12986,17 +12988,17 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="18" spans="19:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S18" s="42" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="19:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S20" s="33" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="19:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="19:23" x14ac:dyDescent="0.25">
       <c r="T21" s="33" t="s">
         <v>125</v>
       </c>
@@ -13006,7 +13008,7 @@
       </c>
       <c r="W21" s="33"/>
     </row>
-    <row r="22" spans="19:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S22" s="43" t="s">
         <v>131</v>
       </c>
@@ -13023,7 +13025,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="19:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S23" s="38" t="s">
         <v>138</v>
       </c>
@@ -13040,7 +13042,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="24" spans="19:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S24" s="38" t="s">
         <v>142</v>
       </c>
@@ -13053,7 +13055,7 @@
       </c>
       <c r="W24" s="35"/>
     </row>
-    <row r="25" spans="19:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S25" s="38" t="s">
         <v>149</v>
       </c>
@@ -13070,7 +13072,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="26" spans="19:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S26" s="42" t="s">
         <v>151</v>
       </c>
@@ -13090,15 +13092,15 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" customWidth="1"/>
-    <col min="6" max="7" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>164</v>
       </c>
@@ -13115,7 +13117,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>169</v>
       </c>
@@ -13162,7 +13164,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="47">
         <v>1</v>
       </c>
@@ -13210,7 +13212,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>182</v>
       </c>
@@ -13252,7 +13254,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>184</v>
       </c>
@@ -13285,7 +13287,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>184</v>
       </c>
@@ -13315,7 +13317,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>184</v>
       </c>
@@ -13336,7 +13338,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>184</v>
       </c>
@@ -13363,7 +13365,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>184</v>
       </c>
@@ -13391,7 +13393,7 @@
         <v>0.13824884792626729</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>184</v>
       </c>
@@ -13416,7 +13418,7 @@
         <v>9.8360655737704916E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>184</v>
       </c>
@@ -13434,19 +13436,19 @@
         <v>7.6E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="50"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="50"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="50"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
         <v>190</v>
       </c>

</xml_diff>